<commit_message>
Fixed Category and Explicit wait issue
</commit_message>
<xml_diff>
--- a/DataFolder/IPPB_Manager_Select_EMP.xlsx
+++ b/DataFolder/IPPB_Manager_Select_EMP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\USRLocalization\DataFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2744CDA3-7316-451B-AFFA-39DD44FEBB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F22903-1843-4451-AC0B-79FBDFDB48C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,121 +25,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Empoyee name</t>
   </si>
   <si>
-    <t>USR101966</t>
-  </si>
-  <si>
-    <t>USR101967</t>
-  </si>
-  <si>
-    <t>USR101968</t>
-  </si>
-  <si>
-    <t>USR101969</t>
-  </si>
-  <si>
-    <t>USR101970</t>
-  </si>
-  <si>
-    <t>USR101971</t>
-  </si>
-  <si>
-    <t>USR101972</t>
-  </si>
-  <si>
-    <t>USR101973</t>
-  </si>
-  <si>
-    <t>USR101974</t>
-  </si>
-  <si>
-    <t>USR101975</t>
-  </si>
-  <si>
-    <t>USR101976</t>
-  </si>
-  <si>
-    <t>USR101977</t>
-  </si>
-  <si>
-    <t>USR101978</t>
-  </si>
-  <si>
-    <t>USR101979</t>
-  </si>
-  <si>
-    <t>USR101980</t>
-  </si>
-  <si>
-    <t>USR101981</t>
-  </si>
-  <si>
-    <t>USR101982</t>
-  </si>
-  <si>
-    <t>USR101983</t>
-  </si>
-  <si>
-    <t>USR101984</t>
-  </si>
-  <si>
-    <t>USR101985</t>
-  </si>
-  <si>
-    <t>USR101986</t>
-  </si>
-  <si>
-    <t>USR101987</t>
-  </si>
-  <si>
-    <t>USR101988</t>
-  </si>
-  <si>
-    <t>USR101989</t>
-  </si>
-  <si>
-    <t>USR101990</t>
-  </si>
-  <si>
-    <t>USR101991</t>
-  </si>
-  <si>
-    <t>USR101992</t>
-  </si>
-  <si>
-    <t>USR101993</t>
-  </si>
-  <si>
-    <t>USR101994</t>
-  </si>
-  <si>
-    <t>USR101995</t>
-  </si>
-  <si>
-    <t>USR101996</t>
-  </si>
-  <si>
-    <t>USR101997</t>
-  </si>
-  <si>
-    <t>USR101998</t>
-  </si>
-  <si>
-    <t>USR101999</t>
-  </si>
-  <si>
-    <t>USR102000</t>
+    <t>PMS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +48,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -169,27 +73,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -199,8 +88,8 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -536,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A36"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,176 +447,17 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
+      <c r="A3" s="2">
+        <v>526</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>35</v>
+      <c r="A4" s="2">
+        <v>527</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Overall comment in EMP and MGR
</commit_message>
<xml_diff>
--- a/DataFolder/IPPB_Manager_Select_EMP.xlsx
+++ b/DataFolder/IPPB_Manager_Select_EMP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\USRLocalization-main\DataFolder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\USRLocalization\DataFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD0064A1-8061-4C27-B417-F8FC400C39EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{295F620F-9BDD-4806-A81F-E548352667DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,160 +25,310 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
   <si>
     <t>Empoyee ID</t>
   </si>
   <si>
-    <t>USR101704</t>
-  </si>
-  <si>
-    <t>USR101705</t>
-  </si>
-  <si>
-    <t>USR101706</t>
-  </si>
-  <si>
-    <t>USR101707</t>
-  </si>
-  <si>
-    <t>USR101708</t>
-  </si>
-  <si>
-    <t>USR101709</t>
-  </si>
-  <si>
-    <t>USR101710</t>
-  </si>
-  <si>
-    <t>USR101711</t>
-  </si>
-  <si>
-    <t>USR101712</t>
-  </si>
-  <si>
-    <t>USR101713</t>
-  </si>
-  <si>
-    <t>USR101714</t>
-  </si>
-  <si>
-    <t>USR101715</t>
-  </si>
-  <si>
-    <t>USR101716</t>
-  </si>
-  <si>
-    <t>USR101717</t>
-  </si>
-  <si>
-    <t>USR101718</t>
-  </si>
-  <si>
-    <t>USR101719</t>
-  </si>
-  <si>
-    <t>USR101720</t>
-  </si>
-  <si>
-    <t>USR101721</t>
-  </si>
-  <si>
-    <t>USR101722</t>
-  </si>
-  <si>
-    <t>USR101723</t>
-  </si>
-  <si>
-    <t>USR101724</t>
-  </si>
-  <si>
-    <t>USR101725</t>
-  </si>
-  <si>
-    <t>USR101726</t>
-  </si>
-  <si>
-    <t>USR101727</t>
-  </si>
-  <si>
-    <t>USR101728</t>
-  </si>
-  <si>
-    <t>USR101729</t>
-  </si>
-  <si>
-    <t>USR101730</t>
-  </si>
-  <si>
-    <t>USR101731</t>
-  </si>
-  <si>
-    <t>USR101732</t>
-  </si>
-  <si>
-    <t>USR101733</t>
-  </si>
-  <si>
-    <t>USR101734</t>
-  </si>
-  <si>
-    <t>USR101735</t>
-  </si>
-  <si>
-    <t>USR101736</t>
-  </si>
-  <si>
-    <t>USR101737</t>
-  </si>
-  <si>
-    <t>USR101738</t>
-  </si>
-  <si>
-    <t>USR101739</t>
-  </si>
-  <si>
-    <t>USR101740</t>
-  </si>
-  <si>
-    <t>USR101741</t>
-  </si>
-  <si>
-    <t>USR101742</t>
-  </si>
-  <si>
-    <t>USR101743</t>
-  </si>
-  <si>
-    <t>USR101744</t>
-  </si>
-  <si>
-    <t>USR101745</t>
-  </si>
-  <si>
-    <t>USR101746</t>
-  </si>
-  <si>
-    <t>USR101747</t>
-  </si>
-  <si>
-    <t>USR101748</t>
-  </si>
-  <si>
-    <t>USR101749</t>
-  </si>
-  <si>
-    <t>USR101750</t>
-  </si>
-  <si>
-    <t>USR101751</t>
+    <t>USR101565</t>
+  </si>
+  <si>
+    <t>USR101566</t>
+  </si>
+  <si>
+    <t>USR101567</t>
+  </si>
+  <si>
+    <t>USR101568</t>
+  </si>
+  <si>
+    <t>USR101569</t>
+  </si>
+  <si>
+    <t>USR101570</t>
+  </si>
+  <si>
+    <t>USR101571</t>
+  </si>
+  <si>
+    <t>USR101572</t>
+  </si>
+  <si>
+    <t>USR101573</t>
+  </si>
+  <si>
+    <t>USR101574</t>
+  </si>
+  <si>
+    <t>USR101575</t>
+  </si>
+  <si>
+    <t>USR101576</t>
+  </si>
+  <si>
+    <t>USR101577</t>
+  </si>
+  <si>
+    <t>USR101578</t>
+  </si>
+  <si>
+    <t>USR101579</t>
+  </si>
+  <si>
+    <t>USR101580</t>
+  </si>
+  <si>
+    <t>USR101581</t>
+  </si>
+  <si>
+    <t>USR101582</t>
+  </si>
+  <si>
+    <t>USR101583</t>
+  </si>
+  <si>
+    <t>USR101584</t>
+  </si>
+  <si>
+    <t>USR101585</t>
+  </si>
+  <si>
+    <t>USR101586</t>
+  </si>
+  <si>
+    <t>USR101587</t>
+  </si>
+  <si>
+    <t>USR101588</t>
+  </si>
+  <si>
+    <t>USR101589</t>
+  </si>
+  <si>
+    <t>USR101590</t>
+  </si>
+  <si>
+    <t>USR101591</t>
+  </si>
+  <si>
+    <t>USR101592</t>
+  </si>
+  <si>
+    <t>USR101593</t>
+  </si>
+  <si>
+    <t>USR101594</t>
+  </si>
+  <si>
+    <t>USR101595</t>
+  </si>
+  <si>
+    <t>USR101596</t>
+  </si>
+  <si>
+    <t>USR101597</t>
+  </si>
+  <si>
+    <t>USR101598</t>
+  </si>
+  <si>
+    <t>USR101599</t>
+  </si>
+  <si>
+    <t>USR101560</t>
+  </si>
+  <si>
+    <t>USR101561</t>
+  </si>
+  <si>
+    <t>USR101562</t>
+  </si>
+  <si>
+    <t>USR101563</t>
+  </si>
+  <si>
+    <t>USR101564</t>
+  </si>
+  <si>
+    <t>USR101548</t>
+  </si>
+  <si>
+    <t>USR101549</t>
+  </si>
+  <si>
+    <t>USR101550</t>
+  </si>
+  <si>
+    <t>USR101551</t>
+  </si>
+  <si>
+    <t>USR101552</t>
+  </si>
+  <si>
+    <t>USR101553</t>
+  </si>
+  <si>
+    <t>USR101554</t>
+  </si>
+  <si>
+    <t>USR101555</t>
+  </si>
+  <si>
+    <t>USR101556</t>
+  </si>
+  <si>
+    <t>USR101557</t>
+  </si>
+  <si>
+    <t>USR101558</t>
+  </si>
+  <si>
+    <t>USR101559</t>
+  </si>
+  <si>
+    <t>USR101502</t>
+  </si>
+  <si>
+    <t>USR101503</t>
+  </si>
+  <si>
+    <t>USR101504</t>
+  </si>
+  <si>
+    <t>USR101505</t>
+  </si>
+  <si>
+    <t>USR101506</t>
+  </si>
+  <si>
+    <t>USR101507</t>
+  </si>
+  <si>
+    <t>USR101508</t>
+  </si>
+  <si>
+    <t>USR101509</t>
+  </si>
+  <si>
+    <t>USR101510</t>
+  </si>
+  <si>
+    <t>USR101511</t>
+  </si>
+  <si>
+    <t>USR101512</t>
+  </si>
+  <si>
+    <t>USR101513</t>
+  </si>
+  <si>
+    <t>USR101514</t>
+  </si>
+  <si>
+    <t>USR101515</t>
+  </si>
+  <si>
+    <t>USR101516</t>
+  </si>
+  <si>
+    <t>USR101517</t>
+  </si>
+  <si>
+    <t>USR101518</t>
+  </si>
+  <si>
+    <t>USR101519</t>
+  </si>
+  <si>
+    <t>USR101520</t>
+  </si>
+  <si>
+    <t>USR101521</t>
+  </si>
+  <si>
+    <t>USR101522</t>
+  </si>
+  <si>
+    <t>USR101523</t>
+  </si>
+  <si>
+    <t>USR101524</t>
+  </si>
+  <si>
+    <t>USR101525</t>
+  </si>
+  <si>
+    <t>USR101526</t>
+  </si>
+  <si>
+    <t>USR101527</t>
+  </si>
+  <si>
+    <t>USR101528</t>
+  </si>
+  <si>
+    <t>USR101529</t>
+  </si>
+  <si>
+    <t>USR101530</t>
+  </si>
+  <si>
+    <t>USR101531</t>
+  </si>
+  <si>
+    <t>USR101532</t>
+  </si>
+  <si>
+    <t>USR101533</t>
+  </si>
+  <si>
+    <t>USR101534</t>
+  </si>
+  <si>
+    <t>USR101535</t>
+  </si>
+  <si>
+    <t>USR101536</t>
+  </si>
+  <si>
+    <t>USR101537</t>
+  </si>
+  <si>
+    <t>USR101538</t>
+  </si>
+  <si>
+    <t>USR101539</t>
+  </si>
+  <si>
+    <t>USR101540</t>
+  </si>
+  <si>
+    <t>USR101541</t>
+  </si>
+  <si>
+    <t>USR101542</t>
+  </si>
+  <si>
+    <t>USR101543</t>
+  </si>
+  <si>
+    <t>USR101544</t>
+  </si>
+  <si>
+    <t>USR101545</t>
+  </si>
+  <si>
+    <t>USR101546</t>
+  </si>
+  <si>
+    <t>USR101547</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,6 +349,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -214,27 +371,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -244,9 +386,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A77"/>
+  <dimension ref="A1:A99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,327 +739,493 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>16</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>17</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>19</v>
+        <v>71</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>20</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>21</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>23</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>24</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>25</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>26</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>27</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>33</v>
+        <v>85</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>34</v>
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>36</v>
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>38</v>
+        <v>90</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>39</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>41</v>
+        <v>93</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>42</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>43</v>
+        <v>95</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="2"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="2"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="2"/>
-    </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
+      <c r="A56" s="2" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="2"/>
+      <c r="A57" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="2"/>
+      <c r="A58" s="2" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="2"/>
+      <c r="A59" s="2" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="2"/>
+      <c r="A60" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="2"/>
+      <c r="A61" s="2" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="2"/>
+      <c r="A62" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="2"/>
+      <c r="A63" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="2"/>
+      <c r="A64" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="2"/>
+      <c r="A65" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
+      <c r="A66" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="2"/>
+      <c r="A67" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="2"/>
+      <c r="A68" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="2"/>
+      <c r="A69" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="2"/>
+      <c r="A70" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="2"/>
+      <c r="A71" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="2"/>
+      <c r="A72" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="2"/>
+      <c r="A73" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="2"/>
+      <c r="A74" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="2"/>
+      <c r="A75" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="2"/>
+      <c r="A76" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="2"/>
+      <c r="A77" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>